<commit_message>
2021-12-03 add the FID metric
</commit_message>
<xml_diff>
--- a/Test/SRROOT/Set5/AllMetrics.xlsx
+++ b/Test/SRROOT/Set5/AllMetrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ImgName\Metrics</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>LPIPS</t>
+  </si>
+  <si>
+    <t>FID</t>
+  </si>
+  <si>
+    <t>Paq2Piq</t>
   </si>
   <si>
     <t>baby.png</t>
@@ -431,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,10 +486,16 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>33.65387895684216</v>
@@ -524,10 +536,16 @@
       <c r="N2">
         <v>0.2474126666784286</v>
       </c>
+      <c r="O2">
+        <v>29.4329585126558</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>34.606659854964</v>
@@ -568,10 +586,16 @@
       <c r="N3">
         <v>0.06807722151279449</v>
       </c>
+      <c r="O3">
+        <v>22.31222986630225</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>28.43567997375774</v>
@@ -612,10 +636,16 @@
       <c r="N4">
         <v>0.114445723593235</v>
       </c>
+      <c r="O4">
+        <v>58.43144240361824</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>32.70994842175978</v>
@@ -656,10 +686,16 @@
       <c r="N5">
         <v>0.3247846662998199</v>
       </c>
+      <c r="O5">
+        <v>86.8405846731801</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>30.42180878697796</v>
@@ -700,10 +736,16 @@
       <c r="N6">
         <v>0.1403834074735641</v>
       </c>
+      <c r="O6">
+        <v>92.32639214517206</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>31.9656</v>
@@ -743,6 +785,12 @@
       </c>
       <c r="N7">
         <v>0.1790207371115685</v>
+      </c>
+      <c r="O7">
+        <v>57.86872152018569</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>